<commit_message>
release ZRADTri Rev B
</commit_message>
<xml_diff>
--- a/hardware/ZRADTri/ZRADTriBOM.xlsx
+++ b/hardware/ZRADTri/ZRADTriBOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eric\Documents\GitHub\ZRAD\hardware\ZRADTri\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DCCC905-5BE4-407A-8D62-0CC1EF60551D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A63309-4534-43BC-8ADF-E85CEB72929C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24765" yWindow="795" windowWidth="22575" windowHeight="14685" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24600" yWindow="240" windowWidth="22575" windowHeight="14685" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="227">
   <si>
     <t>Item #</t>
   </si>
@@ -252,15 +252,6 @@
     <t>D1</t>
   </si>
   <si>
-    <t>QLSP14RGB_B</t>
-  </si>
-  <si>
-    <t>Quelighting</t>
-  </si>
-  <si>
-    <t>RGB LED</t>
-  </si>
-  <si>
     <t>D2</t>
   </si>
   <si>
@@ -648,9 +639,6 @@
     <t>Cap 120pF 0402 C0G NP0</t>
   </si>
   <si>
-    <t>3970-QLSP14RGB_BCT-ND</t>
-  </si>
-  <si>
     <t>F2715CT-ND</t>
   </si>
   <si>
@@ -741,9 +729,6 @@
     <t>LED Light Pipe 5mm .125"</t>
   </si>
   <si>
-    <t xml:space="preserve">Optional - makes the LED much more visible </t>
-  </si>
-  <si>
     <t>350-4283-ND</t>
   </si>
   <si>
@@ -766,6 +751,27 @@
   </si>
   <si>
     <t>PCB antenna - values TBD</t>
+  </si>
+  <si>
+    <t>Optional - makes the LED much more visible - 5/32 or 4mm hole</t>
+  </si>
+  <si>
+    <t>BL-HJXGXBX32M-D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RGB LED 3.2x2.8mm </t>
+  </si>
+  <si>
+    <t>BL-HJXGXBX32M-DCT-ND</t>
+  </si>
+  <si>
+    <t>Changed RGB LED to 3.2x2.8mm size which is more common</t>
+  </si>
+  <si>
+    <t>CAUTION! Carefully choose alternates as there are many flavors of pinouts!</t>
+  </si>
+  <si>
+    <t>American Bright Optoelectronics Corp</t>
   </si>
 </sst>
 </file>
@@ -1441,7 +1447,7 @@
                   <c:v>1.22</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.1940000000000008</c:v>
+                  <c:v>5.2739999999999991</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2378,10 +2384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2391,40 +2397,40 @@
   <sheetData>
     <row r="1" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="J5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -2445,7 +2451,7 @@
         <v>45406</v>
       </c>
       <c r="B14" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -2453,7 +2459,7 @@
         <v>45455</v>
       </c>
       <c r="B15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -2461,7 +2467,7 @@
         <v>45763</v>
       </c>
       <c r="B16" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -2469,7 +2475,15 @@
         <v>45790</v>
       </c>
       <c r="B17" t="s">
-        <v>220</v>
+        <v>215</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>45839</v>
+      </c>
+      <c r="B18" t="s">
+        <v>224</v>
       </c>
     </row>
   </sheetData>
@@ -2486,7 +2500,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2548,10 +2562,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>10</v>
@@ -2560,7 +2574,7 @@
         <v>29</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="G2" s="10">
         <v>1</v>
@@ -2592,7 +2606,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>9</v>
@@ -2604,7 +2618,7 @@
         <v>33</v>
       </c>
       <c r="F3" s="32" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G3" s="10">
         <v>1</v>
@@ -2624,7 +2638,7 @@
         <v>10</v>
       </c>
       <c r="R3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -2665,10 +2679,10 @@
         <v>10</v>
       </c>
       <c r="R4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="S4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -2709,7 +2723,7 @@
         <v>10</v>
       </c>
       <c r="M5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="R5" t="str">
         <f>$D$2</f>
@@ -2726,19 +2740,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>40</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>45</v>
       </c>
       <c r="F6" s="28" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="G6" s="10">
         <v>1</v>
@@ -2756,7 +2770,7 @@
         <v>10</v>
       </c>
       <c r="M6" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="R6" t="str">
         <f>$D$3</f>
@@ -2782,10 +2796,10 @@
         <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F7" s="28" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="G7" s="10">
         <v>4</v>
@@ -2817,19 +2831,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>40</v>
       </c>
       <c r="D8" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="E8" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>162</v>
-      </c>
       <c r="F8" s="28" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G8" s="10">
         <v>2</v>
@@ -2870,10 +2884,10 @@
         <v>44</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="G9" s="10">
         <v>0</v>
@@ -2891,7 +2905,7 @@
         <v>0</v>
       </c>
       <c r="M9" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="R9" t="str">
         <f>$D$18</f>
@@ -2908,19 +2922,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="40" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>40</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="G10" s="10">
         <v>2</v>
@@ -2938,11 +2952,11 @@
         <v>20</v>
       </c>
       <c r="R10" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="S10" s="2">
         <f>I43-SUM(S5:S9)</f>
-        <v>5.1940000000000008</v>
+        <v>5.2739999999999991</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -2951,19 +2965,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="40" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>40</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G11" s="10">
         <v>1</v>
@@ -2981,11 +2995,11 @@
         <v>10</v>
       </c>
       <c r="R11" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="S11" s="2">
         <f>SUM(S5:S10)</f>
-        <v>16.874000000000002</v>
+        <v>16.954000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="30" x14ac:dyDescent="0.25">
@@ -3000,13 +3014,13 @@
         <v>40</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E12" s="41" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="G12" s="10">
         <v>5</v>
@@ -3039,10 +3053,10 @@
         <v>48</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="G13" s="10">
         <v>4</v>
@@ -3063,19 +3077,19 @@
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="21"/>
       <c r="B14" s="40" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>40</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="G14" s="10">
         <v>2</v>
@@ -3108,10 +3122,10 @@
         <v>51</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="G15" s="10">
         <v>1</v>
@@ -3135,29 +3149,29 @@
         <v>14</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>53</v>
+        <v>221</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>54</v>
+        <v>226</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>55</v>
+        <v>222</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>52</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>185</v>
+        <v>223</v>
       </c>
       <c r="G16" s="10">
         <v>1</v>
       </c>
       <c r="H16" s="11">
-        <v>0.09</v>
+        <v>0.17</v>
       </c>
       <c r="I16" s="11">
         <f t="shared" si="0"/>
-        <v>0.09</v>
+        <v>0.17</v>
       </c>
       <c r="J16" s="9"/>
       <c r="K16" s="12">
@@ -3165,7 +3179,10 @@
         <v>10</v>
       </c>
       <c r="M16" t="s">
-        <v>69</v>
+        <v>66</v>
+      </c>
+      <c r="N16" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -3174,19 +3191,19 @@
         <v>15</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="G17" s="10">
         <v>1</v>
@@ -3210,19 +3227,19 @@
         <v>16</v>
       </c>
       <c r="B18" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" s="9" t="s">
         <v>61</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>64</v>
       </c>
       <c r="G18" s="10">
         <v>1</v>
@@ -3246,19 +3263,19 @@
         <v>17</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="G19" s="10">
         <v>1</v>
@@ -3276,7 +3293,7 @@
         <v>10</v>
       </c>
       <c r="M19" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -3285,19 +3302,19 @@
         <v>18</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>40</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="G20" s="10">
         <v>1</v>
@@ -3318,19 +3335,19 @@
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="21"/>
       <c r="B21" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G21" s="10">
         <v>1</v>
@@ -3354,19 +3371,19 @@
         <v>19</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>40</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="G22" s="10">
         <v>1</v>
@@ -3390,19 +3407,19 @@
         <v>20</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>40</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="G23" s="10">
         <v>2</v>
@@ -3426,19 +3443,19 @@
         <v>21</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>40</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="G24" s="10">
         <v>2</v>
@@ -3462,19 +3479,19 @@
         <v>22</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="G25" s="10">
         <v>1</v>
@@ -3498,19 +3515,19 @@
         <v>23</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>40</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G26" s="10">
         <v>1</v>
@@ -3534,19 +3551,19 @@
         <v>24</v>
       </c>
       <c r="B27" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F27" s="9" t="s">
         <v>75</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="F27" s="9" t="s">
-        <v>78</v>
       </c>
       <c r="G27" s="10">
         <v>2</v>
@@ -3570,19 +3587,19 @@
         <v>25</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G28" s="10">
         <v>2</v>
@@ -3606,19 +3623,19 @@
         <v>26</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G29" s="10">
         <v>1</v>
@@ -3642,19 +3659,19 @@
         <v>27</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G30" s="10">
         <v>1</v>
@@ -3678,19 +3695,19 @@
         <v>28</v>
       </c>
       <c r="B31" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F31" s="9" t="s">
         <v>88</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="F31" s="9" t="s">
-        <v>91</v>
       </c>
       <c r="G31" s="10">
         <v>1</v>
@@ -3714,19 +3731,19 @@
         <v>29</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G32" s="10">
         <v>2</v>
@@ -3750,19 +3767,19 @@
         <v>30</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G33" s="10">
         <v>1</v>
@@ -3786,19 +3803,19 @@
         <v>31</v>
       </c>
       <c r="B34" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="F34" s="9" t="s">
         <v>98</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>211</v>
-      </c>
-      <c r="F34" s="9" t="s">
-        <v>101</v>
       </c>
       <c r="G34" s="10">
         <v>1</v>
@@ -3816,7 +3833,7 @@
         <v>10</v>
       </c>
       <c r="M34" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
@@ -3851,11 +3868,11 @@
         <v>1</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C37" s="9"/>
       <c r="D37" s="9" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E37" s="14"/>
       <c r="F37" s="9"/>
@@ -3872,7 +3889,7 @@
       <c r="J37" s="9"/>
       <c r="K37" s="12"/>
       <c r="M37" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
@@ -3881,15 +3898,15 @@
         <v>2</v>
       </c>
       <c r="B38" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C38" s="9"/>
       <c r="D38" s="9" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E38" s="9"/>
       <c r="F38" s="25" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G38" s="10">
         <v>1</v>
@@ -3904,7 +3921,7 @@
       <c r="J38" s="9"/>
       <c r="K38" s="12"/>
       <c r="M38" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
@@ -3913,17 +3930,17 @@
         <v>3</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E39" s="9"/>
       <c r="F39" s="9" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="G39" s="10">
         <v>1</v>
@@ -3944,17 +3961,17 @@
         <v>4</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="E40" s="9"/>
       <c r="F40" s="25" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="G40" s="10">
         <v>0</v>
@@ -3969,7 +3986,7 @@
       <c r="J40" s="9"/>
       <c r="K40" s="12"/>
       <c r="M40" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
@@ -3980,7 +3997,7 @@
       <c r="B41" s="9"/>
       <c r="C41" s="9"/>
       <c r="D41" s="9" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E41" s="9"/>
       <c r="F41" s="9"/>
@@ -3998,7 +4015,7 @@
       <c r="B42" s="9"/>
       <c r="C42" s="9"/>
       <c r="D42" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E42" s="9"/>
       <c r="F42" s="35"/>
@@ -4018,18 +4035,18 @@
       <c r="D43" s="9"/>
       <c r="E43" s="9"/>
       <c r="F43" s="37" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G43" s="38"/>
       <c r="H43" s="39"/>
       <c r="I43" s="34">
         <f>SUM(I2:I42)</f>
-        <v>16.874000000000002</v>
+        <v>16.954000000000001</v>
       </c>
       <c r="J43" s="9"/>
       <c r="K43" s="12"/>
       <c r="M43" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
@@ -4048,7 +4065,7 @@
       <c r="J44" s="9"/>
       <c r="K44" s="12"/>
       <c r="M44" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
@@ -4067,7 +4084,7 @@
       <c r="J45" s="16"/>
       <c r="K45" s="19"/>
       <c r="M45" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -4195,7 +4212,7 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -4318,7 +4335,7 @@
         <v>4</v>
       </c>
       <c r="I7" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -4538,15 +4555,15 @@
       </c>
       <c r="B15" t="str">
         <f>ZRADTriBOM!B16</f>
-        <v>QLSP14RGB_B</v>
+        <v>BL-HJXGXBX32M-D</v>
       </c>
       <c r="C15" t="str">
         <f>ZRADTriBOM!C16</f>
-        <v>Quelighting</v>
+        <v>American Bright Optoelectronics Corp</v>
       </c>
       <c r="D15" t="str">
         <f>ZRADTriBOM!D16</f>
-        <v>RGB LED</v>
+        <v xml:space="preserve">RGB LED 3.2x2.8mm </v>
       </c>
       <c r="E15" t="str">
         <f>ZRADTriBOM!E16</f>
@@ -4554,7 +4571,7 @@
       </c>
       <c r="F15" t="str">
         <f>ZRADTriBOM!F16</f>
-        <v>3970-QLSP14RGB_BCT-ND</v>
+        <v>BL-HJXGXBX32M-DCT-ND</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -5394,7 +5411,7 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -5517,7 +5534,7 @@
         <v>4</v>
       </c>
       <c r="I7" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -5737,15 +5754,15 @@
       </c>
       <c r="B15" t="str">
         <f>ZRADTriBOM!B16</f>
-        <v>QLSP14RGB_B</v>
+        <v>BL-HJXGXBX32M-D</v>
       </c>
       <c r="C15" t="str">
         <f>ZRADTriBOM!C16</f>
-        <v>Quelighting</v>
+        <v>American Bright Optoelectronics Corp</v>
       </c>
       <c r="D15" t="str">
         <f>ZRADTriBOM!D16</f>
-        <v>RGB LED</v>
+        <v xml:space="preserve">RGB LED 3.2x2.8mm </v>
       </c>
       <c r="E15" t="str">
         <f>ZRADTriBOM!E16</f>
@@ -5753,7 +5770,7 @@
       </c>
       <c r="F15" t="str">
         <f>ZRADTriBOM!F16</f>
-        <v>3970-QLSP14RGB_BCT-ND</v>
+        <v>BL-HJXGXBX32M-DCT-ND</v>
       </c>
       <c r="G15">
         <v>1</v>
@@ -6297,7 +6314,7 @@
         <v>1</v>
       </c>
       <c r="I33" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -6593,7 +6610,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -6625,7 +6642,7 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -6778,7 +6795,7 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -6859,7 +6876,7 @@
         <v>Cap 4.7uF 0805</v>
       </c>
       <c r="E12" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F12" t="str">
         <f>ZRADTriBOM!F12</f>
@@ -6934,15 +6951,15 @@
       </c>
       <c r="B15" t="str">
         <f>ZRADTriBOM!B16</f>
-        <v>QLSP14RGB_B</v>
+        <v>BL-HJXGXBX32M-D</v>
       </c>
       <c r="C15" t="str">
         <f>ZRADTriBOM!C16</f>
-        <v>Quelighting</v>
+        <v>American Bright Optoelectronics Corp</v>
       </c>
       <c r="D15" t="str">
         <f>ZRADTriBOM!D16</f>
-        <v>RGB LED</v>
+        <v xml:space="preserve">RGB LED 3.2x2.8mm </v>
       </c>
       <c r="E15" t="str">
         <f>ZRADTriBOM!E16</f>
@@ -6950,7 +6967,7 @@
       </c>
       <c r="F15" t="str">
         <f>ZRADTriBOM!F16</f>
-        <v>3970-QLSP14RGB_BCT-ND</v>
+        <v>BL-HJXGXBX32M-DCT-ND</v>
       </c>
       <c r="G15">
         <v>1</v>
@@ -7388,7 +7405,7 @@
         <v>Res 1.0K ohm 0603 1%</v>
       </c>
       <c r="E30" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F30" t="str">
         <f>ZRADTriBOM!F32</f>
@@ -7487,7 +7504,7 @@
         <v>1</v>
       </c>
       <c r="I33" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -7876,12 +7893,12 @@
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>